<commit_message>
doc: atualização dos docs release01
Atualização do DRE, cronograma e estimativa de tamanho.
</commit_message>
<xml_diff>
--- a/doc/Estimativa de Tamanho.xlsx
+++ b/doc/Estimativa de Tamanho.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>ATIVIDADE</t>
   </si>
@@ -84,12 +84,6 @@
   </si>
   <si>
     <t>[RFS20]</t>
-  </si>
-  <si>
-    <t>[RFS21]</t>
-  </si>
-  <si>
-    <t>[RFS22]</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -465,12 +459,14 @@
         <v>4</v>
       </c>
       <c r="C3" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="D3" s="6"/>
+        <v>3.0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2.0</v>
+      </c>
       <c r="E3" s="6">
-        <f t="shared" ref="E3:E24" si="1">D3-C3</f>
-        <v>-2</v>
+        <f t="shared" ref="E3:E22" si="1">D3-C3</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="4">
@@ -478,12 +474,14 @@
         <v>5</v>
       </c>
       <c r="C4" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="D4" s="6"/>
+        <v>1.5</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1.0</v>
+      </c>
       <c r="E4" s="6">
         <f t="shared" si="1"/>
-        <v>-3</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="5">
@@ -493,10 +491,12 @@
       <c r="C5" s="5">
         <v>1.5</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="5">
+        <v>1.0</v>
+      </c>
       <c r="E5" s="6">
         <f t="shared" si="1"/>
-        <v>-1.5</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="6">
@@ -504,12 +504,12 @@
         <v>7</v>
       </c>
       <c r="C6" s="5">
-        <v>1.5</v>
+        <v>1.0</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6">
         <f t="shared" si="1"/>
-        <v>-1.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7">
@@ -517,12 +517,14 @@
         <v>8</v>
       </c>
       <c r="C7" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="6"/>
+        <v>2.0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2.0</v>
+      </c>
       <c r="E7" s="6">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -532,10 +534,12 @@
       <c r="C8" s="5">
         <v>1.0</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="5">
+        <v>1.0</v>
+      </c>
       <c r="E8" s="6">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -543,12 +547,14 @@
         <v>10</v>
       </c>
       <c r="C9" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="D9" s="6"/>
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1.0</v>
+      </c>
       <c r="E9" s="6">
         <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -556,12 +562,14 @@
         <v>11</v>
       </c>
       <c r="C10" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="D10" s="6"/>
+        <v>1.0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1.0</v>
+      </c>
       <c r="E10" s="6">
         <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -569,12 +577,12 @@
         <v>12</v>
       </c>
       <c r="C11" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="12">
@@ -595,12 +603,12 @@
         <v>14</v>
       </c>
       <c r="C13" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="14">
@@ -621,12 +629,12 @@
         <v>16</v>
       </c>
       <c r="C15" s="5">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="16">
@@ -699,12 +707,12 @@
         <v>22</v>
       </c>
       <c r="C21" s="5">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6">
         <f t="shared" si="1"/>
-        <v>-3</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="22">
@@ -712,56 +720,42 @@
         <v>23</v>
       </c>
       <c r="C22" s="5">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6">
         <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6">
-        <f t="shared" si="1"/>
-        <v>-2</v>
+      <c r="C23" s="9">
+        <f t="shared" ref="C23:E23" si="2">SUM(C3:C22)</f>
+        <v>39</v>
+      </c>
+      <c r="D23" s="9">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="E23" s="10">
+        <f t="shared" si="2"/>
+        <v>-30</v>
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6">
-        <f t="shared" si="1"/>
-        <v>-3</v>
-      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
     </row>
     <row r="25">
-      <c r="B25" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="9">
-        <f t="shared" ref="C25:E25" si="2">SUM(C3:C24)</f>
-        <v>42</v>
-      </c>
-      <c r="D25" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="10">
-        <f t="shared" si="2"/>
-        <v>-42</v>
-      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
     </row>
     <row r="26">
       <c r="B26" s="11"/>
@@ -786,18 +780,6 @@
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
-    </row>
-    <row r="30">
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-    </row>
-    <row r="31">
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
     </row>
   </sheetData>
   <printOptions gridLines="1" horizontalCentered="1"/>

</xml_diff>